<commit_message>
Completed the swag lab order creation scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/xlSheets/backup_xl/swaglab.xlsx
+++ b/src/main/resources/xlSheets/backup_xl/swaglab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-driven\au-datadriven-test\src\main\resources\xlSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-driven\au-datadriven-test\src\main\resources\xlSheets\backup_xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFFA47B-DBC9-49B9-A607-A1B01324940A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16EC3EE-34F7-4D63-B6B6-4F51299D2983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestNames" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Test Name</t>
   </si>
@@ -64,12 +64,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -94,48 +88,18 @@
     <t>PhNumber</t>
   </si>
   <si>
-    <t>Welcome@123</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
-    <t>nil</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Pronoun</t>
-  </si>
-  <si>
-    <t>He / him / his / himself</t>
-  </si>
-  <si>
-    <t>Race</t>
-  </si>
-  <si>
-    <t>Ethinicity</t>
-  </si>
-  <si>
-    <t>Asian</t>
-  </si>
-  <si>
-    <t>Hispanic or Latino</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
-    <t>UserIdentity</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
     <t>14082</t>
   </si>
   <si>
@@ -148,9 +112,6 @@
     <t>Java</t>
   </si>
   <si>
-    <t>ShipMethod</t>
-  </si>
-  <si>
     <t>CardHolderName</t>
   </si>
   <si>
@@ -163,117 +124,30 @@
     <t>CVV</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
     <t>12/30</t>
   </si>
   <si>
     <t>01/03/1998</t>
   </si>
   <si>
-    <t>nancy</t>
-  </si>
-  <si>
     <t>BuildingNumber</t>
   </si>
   <si>
-    <t>ParticipantType</t>
-  </si>
-  <si>
-    <t>Independent Senior Citizen</t>
-  </si>
-  <si>
-    <t>AU_UI_eMEdBAT_001</t>
-  </si>
-  <si>
-    <t>AU_UI_eMEdBAT_002</t>
-  </si>
-  <si>
-    <t>Welcome@124</t>
-  </si>
-  <si>
-    <t>ResetPassword</t>
-  </si>
-  <si>
     <t>ScenarioTitle</t>
   </si>
   <si>
     <t>3703 Walt Nuzum Farm Road</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Dependent</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>4242 4242 4242 4242</t>
   </si>
   <si>
-    <t>ToWhom</t>
-  </si>
-  <si>
-    <t>CovidReasons</t>
-  </si>
-  <si>
-    <t>0||0</t>
-  </si>
-  <si>
-    <t>VLabQuestion</t>
-  </si>
-  <si>
-    <t>AirlineInfo</t>
-  </si>
-  <si>
-    <t>Y|Y|Y|Y||N|Y|Y</t>
-  </si>
-  <si>
-    <t>Allegiant Air|Australia|Java</t>
-  </si>
-  <si>
-    <t>CorePreFlightQuestion</t>
-  </si>
-  <si>
     <t>Automation</t>
   </si>
   <si>
     <t>QA</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>PurchaseReasons|Due to COVID symptoms</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t>PurchaseReasons</t>
-  </si>
-  <si>
-    <t>Verify the user is able to create an emed account and password reset in eCommerce site.</t>
-  </si>
-  <si>
-    <t>Verify the user is able to purchase a kit and cancel the order in ecommerce site</t>
-  </si>
-  <si>
-    <t>eCommerce Account Creation and Password Reset</t>
-  </si>
-  <si>
-    <t>eCommerce Order Cancelation</t>
-  </si>
-  <si>
-    <t>Welcome@125</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
@@ -281,6 +155,27 @@
   </si>
   <si>
     <t>swaglab</t>
+  </si>
+  <si>
+    <t>SwagLab Order Creation</t>
+  </si>
+  <si>
+    <t>Verify the user is able to purchase a product from swaglab site</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>Muju</t>
+  </si>
+  <si>
+    <t>AU_UI_SwagLab_001</t>
+  </si>
+  <si>
+    <t>AU_UI_SwagLab_002</t>
   </si>
 </sst>
 </file>
@@ -358,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -381,9 +276,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -728,7 +620,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -748,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,34 +652,21 @@
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" customWidth="1"/>
     <col min="6" max="6" width="23.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" customWidth="1"/>
-    <col min="25" max="25" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5546875" customWidth="1"/>
-    <col min="30" max="30" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.88671875" customWidth="1"/>
-    <col min="50" max="50" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.88671875" customWidth="1"/>
+    <col min="34" max="34" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -798,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>8</v>
@@ -807,349 +686,199 @@
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="V1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>60</v>
+      <c r="M2" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="T2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>75</v>
+      <c r="V2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>60</v>
+      <c r="M3" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="T3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL3" s="10" t="s">
-        <v>74</v>
+      <c r="V3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3 C2:C3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Y,N"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" display="Welcome@123" xr:uid="{7CEBB363-0260-4D9E-9AD1-221A2DA357CF}"/>
-    <hyperlink ref="I3" r:id="rId3" display="Welcome@123" xr:uid="{B7ED5DAA-D5B4-4B8D-81AC-69D3C896893A}"/>
-    <hyperlink ref="H3" r:id="rId4" display="Welcome@123" xr:uid="{06F45121-0390-418D-A353-E0ED58F87A31}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>